<commit_message>
Api Automation using HttpClient
</commit_message>
<xml_diff>
--- a/SkillReview_CharanKumar.xlsx
+++ b/SkillReview_CharanKumar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DotNetPractice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00BB8F5-F2D3-407E-81C9-D579DDB602EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDEF1B6-743F-4AEB-B4DB-826335C0E8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1806,6 +1806,21 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1938,6 +1953,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1949,24 +1967,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2509,60 +2509,60 @@
         <v>247</v>
       </c>
       <c r="B1" s="69"/>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="79" t="s">
         <v>243</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="95" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="92"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="97"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="70" t="s">
         <v>248</v>
       </c>
       <c r="B2" s="71"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="95"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="70" t="s">
         <v>249</v>
       </c>
       <c r="B3" s="71"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="95"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="100"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="70" t="s">
         <v>250</v>
       </c>
       <c r="B4" s="71"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="95"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="100"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="72" t="s">
@@ -2571,48 +2571,48 @@
       <c r="B5" s="73" t="s">
         <v>246</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="103"/>
     </row>
     <row r="6" spans="1:10" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="87"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="83"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="85"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="90"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="86" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="88" t="s">
+      <c r="A9" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="93" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="63" t="s">
@@ -2629,8 +2629,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="87"/>
-      <c r="B10" s="89"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="94"/>
       <c r="C10" s="64" t="s">
         <v>8</v>
       </c>
@@ -2645,7 +2645,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="104" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -2669,7 +2669,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="100"/>
+      <c r="A12" s="105"/>
       <c r="B12" s="41" t="s">
         <v>12</v>
       </c>
@@ -2687,7 +2687,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="100"/>
+      <c r="A13" s="105"/>
       <c r="B13" s="41" t="s">
         <v>13</v>
       </c>
@@ -2705,7 +2705,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="100"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="41" t="s">
         <v>14</v>
       </c>
@@ -2723,7 +2723,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="100"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="41" t="s">
         <v>15</v>
       </c>
@@ -2741,7 +2741,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="101"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="3" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +2763,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="101"/>
+      <c r="A17" s="106"/>
       <c r="B17" s="41" t="s">
         <v>17</v>
       </c>
@@ -2781,7 +2781,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="101"/>
+      <c r="A18" s="106"/>
       <c r="B18" s="41" t="s">
         <v>18</v>
       </c>
@@ -2799,7 +2799,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="101"/>
+      <c r="A19" s="106"/>
       <c r="B19" s="41" t="s">
         <v>19</v>
       </c>
@@ -2817,7 +2817,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="101"/>
+      <c r="A20" s="106"/>
       <c r="B20" s="41" t="s">
         <v>20</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="101"/>
+      <c r="A21" s="106"/>
       <c r="B21" s="41" t="s">
         <v>21</v>
       </c>
@@ -2853,7 +2853,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="101"/>
+      <c r="A22" s="106"/>
       <c r="B22" s="41" t="s">
         <v>22</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="101"/>
+      <c r="A23" s="106"/>
       <c r="B23" s="41" t="s">
         <v>23</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="101"/>
+      <c r="A24" s="106"/>
       <c r="B24" s="41" t="s">
         <v>24</v>
       </c>
@@ -2907,7 +2907,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="101"/>
+      <c r="A25" s="106"/>
       <c r="B25" s="41" t="s">
         <v>25</v>
       </c>
@@ -2925,7 +2925,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="102"/>
+      <c r="A26" s="107"/>
       <c r="B26" s="48" t="s">
         <v>26</v>
       </c>
@@ -2943,7 +2943,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="102"/>
+      <c r="A27" s="107"/>
       <c r="B27" s="3" t="s">
         <v>27</v>
       </c>
@@ -2965,7 +2965,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="102"/>
+      <c r="A28" s="107"/>
       <c r="B28" s="41" t="s">
         <v>28</v>
       </c>
@@ -2983,7 +2983,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="102"/>
+      <c r="A29" s="107"/>
       <c r="B29" s="41" t="s">
         <v>29</v>
       </c>
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="102"/>
+      <c r="A30" s="107"/>
       <c r="B30" s="41" t="s">
         <v>30</v>
       </c>
@@ -3019,7 +3019,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="102"/>
+      <c r="A31" s="107"/>
       <c r="B31" s="3" t="s">
         <v>31</v>
       </c>
@@ -3037,7 +3037,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="102"/>
+      <c r="A32" s="107"/>
       <c r="B32" s="41" t="s">
         <v>32</v>
       </c>
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="102"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="41" t="s">
         <v>33</v>
       </c>
@@ -3073,7 +3073,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102"/>
+      <c r="A34" s="107"/>
       <c r="B34" s="41" t="s">
         <v>34</v>
       </c>
@@ -3091,7 +3091,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="102"/>
+      <c r="A35" s="107"/>
       <c r="B35" s="41" t="s">
         <v>35</v>
       </c>
@@ -3109,7 +3109,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="102"/>
+      <c r="A36" s="107"/>
       <c r="B36" s="41" t="s">
         <v>36</v>
       </c>
@@ -3127,7 +3127,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="102"/>
+      <c r="A37" s="107"/>
       <c r="B37" s="3" t="s">
         <v>37</v>
       </c>
@@ -3148,7 +3148,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="102"/>
+      <c r="A38" s="107"/>
       <c r="B38" s="41" t="s">
         <v>38</v>
       </c>
@@ -3166,7 +3166,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="102"/>
+      <c r="A39" s="107"/>
       <c r="B39" s="41" t="s">
         <v>39</v>
       </c>
@@ -3184,7 +3184,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="102"/>
+      <c r="A40" s="107"/>
       <c r="B40" s="41" t="s">
         <v>40</v>
       </c>
@@ -3202,7 +3202,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="102"/>
+      <c r="A41" s="107"/>
       <c r="B41" s="41" t="s">
         <v>41</v>
       </c>
@@ -3220,7 +3220,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="102"/>
+      <c r="A42" s="107"/>
       <c r="B42" s="41" t="s">
         <v>42</v>
       </c>
@@ -3238,7 +3238,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="102"/>
+      <c r="A43" s="107"/>
       <c r="B43" s="3" t="s">
         <v>43</v>
       </c>
@@ -3260,7 +3260,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="103"/>
+      <c r="A44" s="108"/>
       <c r="B44" s="43" t="s">
         <v>44</v>
       </c>
@@ -3278,7 +3278,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="103"/>
+      <c r="A45" s="108"/>
       <c r="B45" s="43" t="s">
         <v>45</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="103"/>
+      <c r="A46" s="108"/>
       <c r="B46" s="43" t="s">
         <v>46</v>
       </c>
@@ -3314,7 +3314,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="103"/>
+      <c r="A47" s="108"/>
       <c r="B47" s="43" t="s">
         <v>47</v>
       </c>
@@ -3332,7 +3332,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="103"/>
+      <c r="A48" s="108"/>
       <c r="B48" s="43" t="s">
         <v>48</v>
       </c>
@@ -3350,7 +3350,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="103"/>
+      <c r="A49" s="108"/>
       <c r="B49" s="43" t="s">
         <v>49</v>
       </c>
@@ -3368,7 +3368,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="103"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="44" t="s">
         <v>50</v>
       </c>
@@ -3390,7 +3390,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="103"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="43" t="s">
         <v>51</v>
       </c>
@@ -3408,7 +3408,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="103"/>
+      <c r="A52" s="108"/>
       <c r="B52" s="43" t="s">
         <v>52</v>
       </c>
@@ -3426,7 +3426,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="104"/>
+      <c r="A53" s="109"/>
       <c r="B53" s="57" t="s">
         <v>53</v>
       </c>
@@ -3444,7 +3444,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="105" t="s">
+      <c r="A54" s="110" t="s">
         <v>54</v>
       </c>
       <c r="B54" s="51" t="s">
@@ -3468,7 +3468,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="102"/>
+      <c r="A55" s="107"/>
       <c r="B55" s="52" t="s">
         <v>56</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="102"/>
+      <c r="A56" s="107"/>
       <c r="B56" s="52" t="s">
         <v>57</v>
       </c>
@@ -3504,7 +3504,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="102"/>
+      <c r="A57" s="107"/>
       <c r="B57" s="52" t="s">
         <v>58</v>
       </c>
@@ -3522,7 +3522,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="102"/>
+      <c r="A58" s="107"/>
       <c r="B58" s="52" t="s">
         <v>59</v>
       </c>
@@ -3540,7 +3540,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="102"/>
+      <c r="A59" s="107"/>
       <c r="B59" s="52" t="s">
         <v>60</v>
       </c>
@@ -3558,7 +3558,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="102"/>
+      <c r="A60" s="107"/>
       <c r="B60" s="52" t="s">
         <v>61</v>
       </c>
@@ -3576,7 +3576,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="102"/>
+      <c r="A61" s="107"/>
       <c r="B61" s="52" t="s">
         <v>62</v>
       </c>
@@ -3594,7 +3594,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="102"/>
+      <c r="A62" s="107"/>
       <c r="B62" s="52" t="s">
         <v>63</v>
       </c>
@@ -3612,7 +3612,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="102"/>
+      <c r="A63" s="107"/>
       <c r="B63" s="52" t="s">
         <v>64</v>
       </c>
@@ -3630,7 +3630,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="102"/>
+      <c r="A64" s="107"/>
       <c r="B64" s="50" t="s">
         <v>65</v>
       </c>
@@ -3652,7 +3652,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="102"/>
+      <c r="A65" s="107"/>
       <c r="B65" s="53" t="s">
         <v>66</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="102"/>
+      <c r="A66" s="107"/>
       <c r="B66" s="53" t="s">
         <v>67</v>
       </c>
@@ -3688,7 +3688,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="102"/>
+      <c r="A67" s="107"/>
       <c r="B67" s="53" t="s">
         <v>68</v>
       </c>
@@ -3706,7 +3706,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="102"/>
+      <c r="A68" s="107"/>
       <c r="B68" s="53" t="s">
         <v>69</v>
       </c>
@@ -3724,7 +3724,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="102"/>
+      <c r="A69" s="107"/>
       <c r="B69" s="53" t="s">
         <v>70</v>
       </c>
@@ -3742,7 +3742,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="102"/>
+      <c r="A70" s="107"/>
       <c r="B70" s="53" t="s">
         <v>71</v>
       </c>
@@ -3760,7 +3760,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="102"/>
+      <c r="A71" s="107"/>
       <c r="B71" s="53" t="s">
         <v>72</v>
       </c>
@@ -3778,7 +3778,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="102"/>
+      <c r="A72" s="107"/>
       <c r="B72" s="50" t="s">
         <v>73</v>
       </c>
@@ -3800,7 +3800,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="102"/>
+      <c r="A73" s="107"/>
       <c r="B73" s="55" t="s">
         <v>74</v>
       </c>
@@ -3818,7 +3818,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="102"/>
+      <c r="A74" s="107"/>
       <c r="B74" s="53" t="s">
         <v>75</v>
       </c>
@@ -3836,7 +3836,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="102"/>
+      <c r="A75" s="107"/>
       <c r="B75" s="53" t="s">
         <v>76</v>
       </c>
@@ -3854,7 +3854,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="102"/>
+      <c r="A76" s="107"/>
       <c r="B76" s="53" t="s">
         <v>77</v>
       </c>
@@ -3872,7 +3872,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="102"/>
+      <c r="A77" s="107"/>
       <c r="B77" s="50" t="s">
         <v>78</v>
       </c>
@@ -3894,7 +3894,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="102"/>
+      <c r="A78" s="107"/>
       <c r="B78" s="53" t="s">
         <v>79</v>
       </c>
@@ -3912,7 +3912,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="102"/>
+      <c r="A79" s="107"/>
       <c r="B79" s="53" t="s">
         <v>80</v>
       </c>
@@ -3930,7 +3930,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="102"/>
+      <c r="A80" s="107"/>
       <c r="B80" s="53" t="s">
         <v>81</v>
       </c>
@@ -3948,7 +3948,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="102"/>
+      <c r="A81" s="107"/>
       <c r="B81" s="53" t="s">
         <v>82</v>
       </c>
@@ -3966,7 +3966,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="102"/>
+      <c r="A82" s="107"/>
       <c r="B82" s="53" t="s">
         <v>83</v>
       </c>
@@ -3984,7 +3984,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="102"/>
+      <c r="A83" s="107"/>
       <c r="B83" s="53" t="s">
         <v>84</v>
       </c>
@@ -4002,7 +4002,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="102"/>
+      <c r="A84" s="107"/>
       <c r="B84" s="53" t="s">
         <v>85</v>
       </c>
@@ -4020,7 +4020,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="102"/>
+      <c r="A85" s="107"/>
       <c r="B85" s="53" t="s">
         <v>86</v>
       </c>
@@ -4038,7 +4038,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="102"/>
+      <c r="A86" s="107"/>
       <c r="B86" s="53" t="s">
         <v>87</v>
       </c>
@@ -4056,7 +4056,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="102"/>
+      <c r="A87" s="107"/>
       <c r="B87" s="50" t="s">
         <v>88</v>
       </c>
@@ -4078,7 +4078,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="102"/>
+      <c r="A88" s="107"/>
       <c r="B88" s="56" t="s">
         <v>89</v>
       </c>
@@ -4096,7 +4096,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="102"/>
+      <c r="A89" s="107"/>
       <c r="B89" s="56" t="s">
         <v>90</v>
       </c>
@@ -4114,7 +4114,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="102"/>
+      <c r="A90" s="107"/>
       <c r="B90" s="56" t="s">
         <v>91</v>
       </c>
@@ -4132,7 +4132,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="102"/>
+      <c r="A91" s="107"/>
       <c r="B91" s="56" t="s">
         <v>92</v>
       </c>
@@ -4150,7 +4150,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="102"/>
+      <c r="A92" s="107"/>
       <c r="B92" s="56" t="s">
         <v>93</v>
       </c>
@@ -4168,7 +4168,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="102"/>
+      <c r="A93" s="107"/>
       <c r="B93" s="56" t="s">
         <v>94</v>
       </c>
@@ -4186,7 +4186,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="102"/>
+      <c r="A94" s="107"/>
       <c r="B94" s="54" t="s">
         <v>95</v>
       </c>
@@ -4206,7 +4206,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="102"/>
+      <c r="A95" s="107"/>
       <c r="B95" s="49" t="s">
         <v>96</v>
       </c>
@@ -4224,7 +4224,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="102"/>
+      <c r="A96" s="107"/>
       <c r="B96" s="49" t="s">
         <v>97</v>
       </c>
@@ -4242,7 +4242,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="102"/>
+      <c r="A97" s="107"/>
       <c r="B97" s="49" t="s">
         <v>98</v>
       </c>
@@ -4260,7 +4260,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="104"/>
+      <c r="A98" s="109"/>
       <c r="B98" s="59" t="s">
         <v>99</v>
       </c>
@@ -4278,7 +4278,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="74" t="s">
+      <c r="A99" s="79" t="s">
         <v>100</v>
       </c>
       <c r="B99" s="30" t="s">
@@ -4302,7 +4302,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="75"/>
+      <c r="A100" s="80"/>
       <c r="B100" s="46" t="s">
         <v>102</v>
       </c>
@@ -4320,7 +4320,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="75"/>
+      <c r="A101" s="80"/>
       <c r="B101" s="46" t="s">
         <v>79</v>
       </c>
@@ -4338,7 +4338,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="75"/>
+      <c r="A102" s="80"/>
       <c r="B102" s="10" t="s">
         <v>103</v>
       </c>
@@ -4360,7 +4360,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="75"/>
+      <c r="A103" s="80"/>
       <c r="B103" s="41" t="s">
         <v>104</v>
       </c>
@@ -4378,7 +4378,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="75"/>
+      <c r="A104" s="80"/>
       <c r="B104" s="41" t="s">
         <v>105</v>
       </c>
@@ -4396,7 +4396,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="75"/>
+      <c r="A105" s="80"/>
       <c r="B105" s="10" t="s">
         <v>106</v>
       </c>
@@ -4418,7 +4418,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="75"/>
+      <c r="A106" s="80"/>
       <c r="B106" s="41" t="s">
         <v>107</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="75"/>
+      <c r="A107" s="80"/>
       <c r="B107" s="41" t="s">
         <v>108</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="75"/>
+      <c r="A108" s="80"/>
       <c r="B108" s="41" t="s">
         <v>109</v>
       </c>
@@ -4472,7 +4472,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="75"/>
+      <c r="A109" s="80"/>
       <c r="B109" s="41" t="s">
         <v>110</v>
       </c>
@@ -4490,7 +4490,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="75"/>
+      <c r="A110" s="80"/>
       <c r="B110" s="10" t="s">
         <v>111</v>
       </c>
@@ -4512,7 +4512,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="75"/>
+      <c r="A111" s="80"/>
       <c r="B111" s="41" t="s">
         <v>112</v>
       </c>
@@ -4530,7 +4530,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="75"/>
+      <c r="A112" s="80"/>
       <c r="B112" s="41" t="s">
         <v>113</v>
       </c>
@@ -4548,7 +4548,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="75"/>
+      <c r="A113" s="80"/>
       <c r="B113" s="41" t="s">
         <v>114</v>
       </c>
@@ -4566,7 +4566,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="75"/>
+      <c r="A114" s="80"/>
       <c r="B114" s="41" t="s">
         <v>115</v>
       </c>
@@ -4584,7 +4584,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="75"/>
+      <c r="A115" s="80"/>
       <c r="B115" s="41" t="s">
         <v>116</v>
       </c>
@@ -4602,7 +4602,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="75"/>
+      <c r="A116" s="80"/>
       <c r="B116" s="10" t="s">
         <v>117</v>
       </c>
@@ -4624,7 +4624,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="75"/>
+      <c r="A117" s="80"/>
       <c r="B117" s="41" t="s">
         <v>118</v>
       </c>
@@ -4642,7 +4642,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="75"/>
+      <c r="A118" s="80"/>
       <c r="B118" s="41" t="s">
         <v>119</v>
       </c>
@@ -4660,7 +4660,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="75"/>
+      <c r="A119" s="80"/>
       <c r="B119" s="41" t="s">
         <v>120</v>
       </c>
@@ -4678,7 +4678,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="75"/>
+      <c r="A120" s="80"/>
       <c r="B120" s="41" t="s">
         <v>121</v>
       </c>
@@ -4696,7 +4696,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="75"/>
+      <c r="A121" s="80"/>
       <c r="B121" s="10" t="s">
         <v>122</v>
       </c>
@@ -4718,7 +4718,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="75"/>
+      <c r="A122" s="80"/>
       <c r="B122" s="43" t="s">
         <v>123</v>
       </c>
@@ -4736,7 +4736,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="75"/>
+      <c r="A123" s="80"/>
       <c r="B123" s="43" t="s">
         <v>124</v>
       </c>
@@ -4754,7 +4754,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="75"/>
+      <c r="A124" s="80"/>
       <c r="B124" s="43" t="s">
         <v>125</v>
       </c>
@@ -4772,7 +4772,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="75"/>
+      <c r="A125" s="80"/>
       <c r="B125" s="43" t="s">
         <v>126</v>
       </c>
@@ -4790,7 +4790,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A126" s="75"/>
+      <c r="A126" s="80"/>
       <c r="B126" s="44" t="s">
         <v>127</v>
       </c>
@@ -4812,7 +4812,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A127" s="75"/>
+      <c r="A127" s="80"/>
       <c r="B127" s="41" t="s">
         <v>128</v>
       </c>
@@ -4830,7 +4830,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A128" s="75"/>
+      <c r="A128" s="80"/>
       <c r="B128" s="41" t="s">
         <v>129</v>
       </c>
@@ -4848,7 +4848,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A129" s="75"/>
+      <c r="A129" s="80"/>
       <c r="B129" s="41" t="s">
         <v>130</v>
       </c>
@@ -4866,7 +4866,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="75"/>
+      <c r="A130" s="80"/>
       <c r="B130" s="41" t="s">
         <v>131</v>
       </c>
@@ -4884,7 +4884,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="75"/>
+      <c r="A131" s="80"/>
       <c r="B131" s="41" t="s">
         <v>132</v>
       </c>
@@ -4902,7 +4902,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="75"/>
+      <c r="A132" s="80"/>
       <c r="B132" s="41" t="s">
         <v>133</v>
       </c>
@@ -4920,7 +4920,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A133" s="76"/>
+      <c r="A133" s="81"/>
       <c r="B133" s="57" t="s">
         <v>134</v>
       </c>
@@ -4938,7 +4938,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="74" t="s">
+      <c r="A134" s="79" t="s">
         <v>135</v>
       </c>
       <c r="B134" s="30" t="s">
@@ -4962,7 +4962,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="75"/>
+      <c r="A135" s="80"/>
       <c r="B135" s="49" t="s">
         <v>137</v>
       </c>
@@ -4980,7 +4980,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="75"/>
+      <c r="A136" s="80"/>
       <c r="B136" s="49" t="s">
         <v>138</v>
       </c>
@@ -4998,7 +4998,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="75"/>
+      <c r="A137" s="80"/>
       <c r="B137" s="49" t="s">
         <v>139</v>
       </c>
@@ -5016,7 +5016,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="75"/>
+      <c r="A138" s="80"/>
       <c r="B138" s="49" t="s">
         <v>140</v>
       </c>
@@ -5034,7 +5034,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="75"/>
+      <c r="A139" s="80"/>
       <c r="B139" s="49" t="s">
         <v>141</v>
       </c>
@@ -5052,7 +5052,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="75"/>
+      <c r="A140" s="80"/>
       <c r="B140" s="3" t="s">
         <v>142</v>
       </c>
@@ -5072,7 +5072,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="75"/>
+      <c r="A141" s="80"/>
       <c r="B141" s="41" t="s">
         <v>143</v>
       </c>
@@ -5090,7 +5090,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="75"/>
+      <c r="A142" s="80"/>
       <c r="B142" s="41" t="s">
         <v>144</v>
       </c>
@@ -5108,7 +5108,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="75"/>
+      <c r="A143" s="80"/>
       <c r="B143" s="41" t="s">
         <v>145</v>
       </c>
@@ -5126,7 +5126,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="75"/>
+      <c r="A144" s="80"/>
       <c r="B144" s="41" t="s">
         <v>146</v>
       </c>
@@ -5144,7 +5144,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="75"/>
+      <c r="A145" s="80"/>
       <c r="B145" s="41" t="s">
         <v>147</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="75"/>
+      <c r="A146" s="80"/>
       <c r="B146" s="41" t="s">
         <v>148</v>
       </c>
@@ -5180,7 +5180,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="75"/>
+      <c r="A147" s="80"/>
       <c r="B147" s="9" t="s">
         <v>149</v>
       </c>
@@ -5202,7 +5202,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="75"/>
+      <c r="A148" s="80"/>
       <c r="B148" s="41" t="s">
         <v>150</v>
       </c>
@@ -5220,7 +5220,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="75"/>
+      <c r="A149" s="80"/>
       <c r="B149" s="41" t="s">
         <v>151</v>
       </c>
@@ -5238,7 +5238,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="75"/>
+      <c r="A150" s="80"/>
       <c r="B150" s="41" t="s">
         <v>152</v>
       </c>
@@ -5256,7 +5256,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A151" s="76"/>
+      <c r="A151" s="81"/>
       <c r="B151" s="57" t="s">
         <v>153</v>
       </c>
@@ -5329,72 +5329,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="82"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88" t="s">
+      <c r="A4" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88" t="s">
+      <c r="H4" s="93"/>
+      <c r="I4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="106"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="87"/>
-      <c r="B5" s="89"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="94"/>
       <c r="C5" s="64" t="s">
         <v>156</v>
       </c>
@@ -5421,7 +5421,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="104" t="s">
         <v>158</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -5457,7 +5457,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="100"/>
+      <c r="A7" s="105"/>
       <c r="B7" s="41" t="s">
         <v>12</v>
       </c>
@@ -5479,7 +5479,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="100"/>
+      <c r="A8" s="105"/>
       <c r="B8" s="41" t="s">
         <v>13</v>
       </c>
@@ -5501,7 +5501,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="100"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="41" t="s">
         <v>14</v>
       </c>
@@ -5523,7 +5523,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="100"/>
+      <c r="A10" s="105"/>
       <c r="B10" s="41" t="s">
         <v>15</v>
       </c>
@@ -5545,7 +5545,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="101"/>
+      <c r="A11" s="106"/>
       <c r="B11" s="3" t="s">
         <v>160</v>
       </c>
@@ -5579,7 +5579,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="101"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="41" t="s">
         <v>161</v>
       </c>
@@ -5601,7 +5601,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="101"/>
+      <c r="A13" s="106"/>
       <c r="B13" s="41" t="s">
         <v>18</v>
       </c>
@@ -5623,7 +5623,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="101"/>
+      <c r="A14" s="106"/>
       <c r="B14" s="41" t="s">
         <v>19</v>
       </c>
@@ -5645,7 +5645,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="101"/>
+      <c r="A15" s="106"/>
       <c r="B15" s="41" t="s">
         <v>20</v>
       </c>
@@ -5667,7 +5667,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="101"/>
+      <c r="A16" s="106"/>
       <c r="B16" s="41" t="s">
         <v>162</v>
       </c>
@@ -5689,7 +5689,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="101"/>
+      <c r="A17" s="106"/>
       <c r="B17" s="41" t="s">
         <v>22</v>
       </c>
@@ -5711,7 +5711,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="101"/>
+      <c r="A18" s="106"/>
       <c r="B18" s="41" t="s">
         <v>23</v>
       </c>
@@ -5733,7 +5733,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="101"/>
+      <c r="A19" s="106"/>
       <c r="B19" s="41" t="s">
         <v>24</v>
       </c>
@@ -5755,7 +5755,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="101"/>
+      <c r="A20" s="106"/>
       <c r="B20" s="41" t="s">
         <v>25</v>
       </c>
@@ -5777,7 +5777,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="102"/>
+      <c r="A21" s="107"/>
       <c r="B21" s="48" t="s">
         <v>26</v>
       </c>
@@ -5799,7 +5799,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="102"/>
+      <c r="A22" s="107"/>
       <c r="B22" s="3" t="s">
         <v>163</v>
       </c>
@@ -5827,7 +5827,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="102"/>
+      <c r="A23" s="107"/>
       <c r="B23" s="41" t="s">
         <v>164</v>
       </c>
@@ -5849,7 +5849,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="102"/>
+      <c r="A24" s="107"/>
       <c r="B24" s="41" t="s">
         <v>165</v>
       </c>
@@ -5871,7 +5871,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="102"/>
+      <c r="A25" s="107"/>
       <c r="B25" s="41" t="s">
         <v>166</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="102"/>
+      <c r="A26" s="107"/>
       <c r="B26" s="41" t="s">
         <v>167</v>
       </c>
@@ -5915,7 +5915,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="102"/>
+      <c r="A27" s="107"/>
       <c r="B27" s="41" t="s">
         <v>168</v>
       </c>
@@ -5937,7 +5937,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="102"/>
+      <c r="A28" s="107"/>
       <c r="B28" s="41" t="s">
         <v>169</v>
       </c>
@@ -5959,7 +5959,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="102"/>
+      <c r="A29" s="107"/>
       <c r="B29" s="3" t="s">
         <v>31</v>
       </c>
@@ -5987,7 +5987,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="102"/>
+      <c r="A30" s="107"/>
       <c r="B30" s="41" t="s">
         <v>32</v>
       </c>
@@ -6009,7 +6009,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="102"/>
+      <c r="A31" s="107"/>
       <c r="B31" s="41" t="s">
         <v>33</v>
       </c>
@@ -6031,7 +6031,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="102"/>
+      <c r="A32" s="107"/>
       <c r="B32" s="41" t="s">
         <v>34</v>
       </c>
@@ -6053,7 +6053,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="102"/>
+      <c r="A33" s="107"/>
       <c r="B33" s="41" t="s">
         <v>35</v>
       </c>
@@ -6075,7 +6075,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102"/>
+      <c r="A34" s="107"/>
       <c r="B34" s="41" t="s">
         <v>36</v>
       </c>
@@ -6097,7 +6097,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="102"/>
+      <c r="A35" s="107"/>
       <c r="B35" s="3" t="s">
         <v>170</v>
       </c>
@@ -6122,7 +6122,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="102"/>
+      <c r="A36" s="107"/>
       <c r="B36" s="41" t="s">
         <v>38</v>
       </c>
@@ -6144,7 +6144,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="102"/>
+      <c r="A37" s="107"/>
       <c r="B37" s="41" t="s">
         <v>39</v>
       </c>
@@ -6166,7 +6166,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="102"/>
+      <c r="A38" s="107"/>
       <c r="B38" s="41" t="s">
         <v>171</v>
       </c>
@@ -6188,7 +6188,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="102"/>
+      <c r="A39" s="107"/>
       <c r="B39" s="41" t="s">
         <v>172</v>
       </c>
@@ -6210,7 +6210,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="102"/>
+      <c r="A40" s="107"/>
       <c r="B40" s="41" t="s">
         <v>41</v>
       </c>
@@ -6232,7 +6232,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="102"/>
+      <c r="A41" s="107"/>
       <c r="B41" s="41" t="s">
         <v>173</v>
       </c>
@@ -6254,7 +6254,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="102"/>
+      <c r="A42" s="107"/>
       <c r="B42" s="3" t="s">
         <v>43</v>
       </c>
@@ -6282,7 +6282,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="103"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="43" t="s">
         <v>44</v>
       </c>
@@ -6304,7 +6304,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="103"/>
+      <c r="A44" s="108"/>
       <c r="B44" s="43" t="s">
         <v>45</v>
       </c>
@@ -6326,7 +6326,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="103"/>
+      <c r="A45" s="108"/>
       <c r="B45" s="43" t="s">
         <v>46</v>
       </c>
@@ -6348,7 +6348,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="103"/>
+      <c r="A46" s="108"/>
       <c r="B46" s="43" t="s">
         <v>47</v>
       </c>
@@ -6370,7 +6370,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="103"/>
+      <c r="A47" s="108"/>
       <c r="B47" s="43" t="s">
         <v>48</v>
       </c>
@@ -6392,7 +6392,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="103"/>
+      <c r="A48" s="108"/>
       <c r="B48" s="43" t="s">
         <v>49</v>
       </c>
@@ -6414,7 +6414,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="103"/>
+      <c r="A49" s="108"/>
       <c r="B49" s="44" t="s">
         <v>50</v>
       </c>
@@ -6444,7 +6444,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="103"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="43" t="s">
         <v>51</v>
       </c>
@@ -6466,7 +6466,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="103"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="43" t="s">
         <v>52</v>
       </c>
@@ -6488,7 +6488,7 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="104"/>
+      <c r="A52" s="109"/>
       <c r="B52" s="57" t="s">
         <v>53</v>
       </c>
@@ -6510,7 +6510,7 @@
       </c>
     </row>
     <row r="53" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="105" t="s">
+      <c r="A53" s="110" t="s">
         <v>54</v>
       </c>
       <c r="B53" s="51" t="s">
@@ -6546,7 +6546,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="102"/>
+      <c r="A54" s="107"/>
       <c r="B54" s="52" t="s">
         <v>56</v>
       </c>
@@ -6568,7 +6568,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="102"/>
+      <c r="A55" s="107"/>
       <c r="B55" s="52" t="s">
         <v>57</v>
       </c>
@@ -6590,7 +6590,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="102"/>
+      <c r="A56" s="107"/>
       <c r="B56" s="52" t="s">
         <v>58</v>
       </c>
@@ -6612,7 +6612,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="102"/>
+      <c r="A57" s="107"/>
       <c r="B57" s="52" t="s">
         <v>59</v>
       </c>
@@ -6634,7 +6634,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="102"/>
+      <c r="A58" s="107"/>
       <c r="B58" s="52" t="s">
         <v>60</v>
       </c>
@@ -6656,7 +6656,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="102"/>
+      <c r="A59" s="107"/>
       <c r="B59" s="52" t="s">
         <v>61</v>
       </c>
@@ -6678,7 +6678,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="102"/>
+      <c r="A60" s="107"/>
       <c r="B60" s="52" t="s">
         <v>62</v>
       </c>
@@ -6700,7 +6700,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="102"/>
+      <c r="A61" s="107"/>
       <c r="B61" s="52" t="s">
         <v>63</v>
       </c>
@@ -6722,7 +6722,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="102"/>
+      <c r="A62" s="107"/>
       <c r="B62" s="52" t="s">
         <v>64</v>
       </c>
@@ -6744,7 +6744,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="102"/>
+      <c r="A63" s="107"/>
       <c r="B63" s="50" t="s">
         <v>65</v>
       </c>
@@ -6774,7 +6774,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="102"/>
+      <c r="A64" s="107"/>
       <c r="B64" s="53" t="s">
         <v>66</v>
       </c>
@@ -6796,7 +6796,7 @@
       </c>
     </row>
     <row r="65" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="102"/>
+      <c r="A65" s="107"/>
       <c r="B65" s="53" t="s">
         <v>67</v>
       </c>
@@ -6818,7 +6818,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="102"/>
+      <c r="A66" s="107"/>
       <c r="B66" s="53" t="s">
         <v>68</v>
       </c>
@@ -6840,7 +6840,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="102"/>
+      <c r="A67" s="107"/>
       <c r="B67" s="53" t="s">
         <v>69</v>
       </c>
@@ -6862,7 +6862,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="102"/>
+      <c r="A68" s="107"/>
       <c r="B68" s="53" t="s">
         <v>70</v>
       </c>
@@ -6884,7 +6884,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="102"/>
+      <c r="A69" s="107"/>
       <c r="B69" s="53" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6906,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="102"/>
+      <c r="A70" s="107"/>
       <c r="B70" s="53" t="s">
         <v>72</v>
       </c>
@@ -6928,7 +6928,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="102"/>
+      <c r="A71" s="107"/>
       <c r="B71" s="50" t="s">
         <v>73</v>
       </c>
@@ -6958,7 +6958,7 @@
       </c>
     </row>
     <row r="72" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="102"/>
+      <c r="A72" s="107"/>
       <c r="B72" s="55" t="s">
         <v>74</v>
       </c>
@@ -6980,7 +6980,7 @@
       </c>
     </row>
     <row r="73" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="102"/>
+      <c r="A73" s="107"/>
       <c r="B73" s="53" t="s">
         <v>75</v>
       </c>
@@ -7002,7 +7002,7 @@
       </c>
     </row>
     <row r="74" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="102"/>
+      <c r="A74" s="107"/>
       <c r="B74" s="53" t="s">
         <v>76</v>
       </c>
@@ -7024,7 +7024,7 @@
       </c>
     </row>
     <row r="75" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="102"/>
+      <c r="A75" s="107"/>
       <c r="B75" s="53" t="s">
         <v>77</v>
       </c>
@@ -7046,7 +7046,7 @@
       </c>
     </row>
     <row r="76" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="102"/>
+      <c r="A76" s="107"/>
       <c r="B76" s="50" t="s">
         <v>78</v>
       </c>
@@ -7080,7 +7080,7 @@
       </c>
     </row>
     <row r="77" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="102"/>
+      <c r="A77" s="107"/>
       <c r="B77" s="53" t="s">
         <v>79</v>
       </c>
@@ -7102,7 +7102,7 @@
       </c>
     </row>
     <row r="78" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="102"/>
+      <c r="A78" s="107"/>
       <c r="B78" s="53" t="s">
         <v>80</v>
       </c>
@@ -7124,7 +7124,7 @@
       </c>
     </row>
     <row r="79" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="102"/>
+      <c r="A79" s="107"/>
       <c r="B79" s="53" t="s">
         <v>81</v>
       </c>
@@ -7146,7 +7146,7 @@
       </c>
     </row>
     <row r="80" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="102"/>
+      <c r="A80" s="107"/>
       <c r="B80" s="53" t="s">
         <v>82</v>
       </c>
@@ -7168,7 +7168,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="102"/>
+      <c r="A81" s="107"/>
       <c r="B81" s="53" t="s">
         <v>83</v>
       </c>
@@ -7190,7 +7190,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="102"/>
+      <c r="A82" s="107"/>
       <c r="B82" s="53" t="s">
         <v>84</v>
       </c>
@@ -7212,7 +7212,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="102"/>
+      <c r="A83" s="107"/>
       <c r="B83" s="53" t="s">
         <v>85</v>
       </c>
@@ -7234,7 +7234,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="102"/>
+      <c r="A84" s="107"/>
       <c r="B84" s="53" t="s">
         <v>86</v>
       </c>
@@ -7256,7 +7256,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="102"/>
+      <c r="A85" s="107"/>
       <c r="B85" s="53" t="s">
         <v>87</v>
       </c>
@@ -7278,7 +7278,7 @@
       </c>
     </row>
     <row r="86" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="102"/>
+      <c r="A86" s="107"/>
       <c r="B86" s="50" t="s">
         <v>88</v>
       </c>
@@ -7310,7 +7310,7 @@
       </c>
     </row>
     <row r="87" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="102"/>
+      <c r="A87" s="107"/>
       <c r="B87" s="56" t="s">
         <v>89</v>
       </c>
@@ -7332,7 +7332,7 @@
       </c>
     </row>
     <row r="88" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="102"/>
+      <c r="A88" s="107"/>
       <c r="B88" s="56" t="s">
         <v>90</v>
       </c>
@@ -7354,7 +7354,7 @@
       </c>
     </row>
     <row r="89" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="102"/>
+      <c r="A89" s="107"/>
       <c r="B89" s="56" t="s">
         <v>91</v>
       </c>
@@ -7376,7 +7376,7 @@
       </c>
     </row>
     <row r="90" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="102"/>
+      <c r="A90" s="107"/>
       <c r="B90" s="56" t="s">
         <v>92</v>
       </c>
@@ -7398,7 +7398,7 @@
       </c>
     </row>
     <row r="91" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="102"/>
+      <c r="A91" s="107"/>
       <c r="B91" s="56" t="s">
         <v>93</v>
       </c>
@@ -7420,7 +7420,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="102"/>
+      <c r="A92" s="107"/>
       <c r="B92" s="56" t="s">
         <v>94</v>
       </c>
@@ -7442,7 +7442,7 @@
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="102"/>
+      <c r="A93" s="107"/>
       <c r="B93" s="54" t="s">
         <v>95</v>
       </c>
@@ -7466,7 +7466,7 @@
       </c>
     </row>
     <row r="94" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="102"/>
+      <c r="A94" s="107"/>
       <c r="B94" s="49" t="s">
         <v>96</v>
       </c>
@@ -7488,7 +7488,7 @@
       </c>
     </row>
     <row r="95" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="102"/>
+      <c r="A95" s="107"/>
       <c r="B95" s="49" t="s">
         <v>97</v>
       </c>
@@ -7510,7 +7510,7 @@
       </c>
     </row>
     <row r="96" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="102"/>
+      <c r="A96" s="107"/>
       <c r="B96" s="49" t="s">
         <v>98</v>
       </c>
@@ -7532,7 +7532,7 @@
       </c>
     </row>
     <row r="97" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="104"/>
+      <c r="A97" s="109"/>
       <c r="B97" s="59" t="s">
         <v>99</v>
       </c>
@@ -7554,7 +7554,7 @@
       </c>
     </row>
     <row r="98" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="74" t="s">
+      <c r="A98" s="79" t="s">
         <v>100</v>
       </c>
       <c r="B98" s="30" t="s">
@@ -7590,7 +7590,7 @@
       </c>
     </row>
     <row r="99" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="75"/>
+      <c r="A99" s="80"/>
       <c r="B99" s="46" t="s">
         <v>102</v>
       </c>
@@ -7612,7 +7612,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="75"/>
+      <c r="A100" s="80"/>
       <c r="B100" s="46" t="s">
         <v>79</v>
       </c>
@@ -7634,7 +7634,7 @@
       </c>
     </row>
     <row r="101" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="75"/>
+      <c r="A101" s="80"/>
       <c r="B101" s="10" t="s">
         <v>103</v>
       </c>
@@ -7668,7 +7668,7 @@
       </c>
     </row>
     <row r="102" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="75"/>
+      <c r="A102" s="80"/>
       <c r="B102" s="41" t="s">
         <v>104</v>
       </c>
@@ -7690,7 +7690,7 @@
       </c>
     </row>
     <row r="103" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="75"/>
+      <c r="A103" s="80"/>
       <c r="B103" s="41" t="s">
         <v>105</v>
       </c>
@@ -7712,7 +7712,7 @@
       </c>
     </row>
     <row r="104" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="75"/>
+      <c r="A104" s="80"/>
       <c r="B104" s="10" t="s">
         <v>106</v>
       </c>
@@ -7746,7 +7746,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="75"/>
+      <c r="A105" s="80"/>
       <c r="B105" s="41" t="s">
         <v>107</v>
       </c>
@@ -7768,7 +7768,7 @@
       </c>
     </row>
     <row r="106" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="75"/>
+      <c r="A106" s="80"/>
       <c r="B106" s="41" t="s">
         <v>108</v>
       </c>
@@ -7790,7 +7790,7 @@
       </c>
     </row>
     <row r="107" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="75"/>
+      <c r="A107" s="80"/>
       <c r="B107" s="41" t="s">
         <v>109</v>
       </c>
@@ -7812,7 +7812,7 @@
       </c>
     </row>
     <row r="108" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="75"/>
+      <c r="A108" s="80"/>
       <c r="B108" s="41" t="s">
         <v>110</v>
       </c>
@@ -7834,7 +7834,7 @@
       </c>
     </row>
     <row r="109" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="75"/>
+      <c r="A109" s="80"/>
       <c r="B109" s="10" t="s">
         <v>111</v>
       </c>
@@ -7864,7 +7864,7 @@
       </c>
     </row>
     <row r="110" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="75"/>
+      <c r="A110" s="80"/>
       <c r="B110" s="41" t="s">
         <v>112</v>
       </c>
@@ -7886,7 +7886,7 @@
       </c>
     </row>
     <row r="111" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="75"/>
+      <c r="A111" s="80"/>
       <c r="B111" s="41" t="s">
         <v>113</v>
       </c>
@@ -7908,7 +7908,7 @@
       </c>
     </row>
     <row r="112" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="75"/>
+      <c r="A112" s="80"/>
       <c r="B112" s="41" t="s">
         <v>114</v>
       </c>
@@ -7930,7 +7930,7 @@
       </c>
     </row>
     <row r="113" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="75"/>
+      <c r="A113" s="80"/>
       <c r="B113" s="41" t="s">
         <v>115</v>
       </c>
@@ -7952,7 +7952,7 @@
       </c>
     </row>
     <row r="114" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="75"/>
+      <c r="A114" s="80"/>
       <c r="B114" s="41" t="s">
         <v>116</v>
       </c>
@@ -7974,7 +7974,7 @@
       </c>
     </row>
     <row r="115" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="75"/>
+      <c r="A115" s="80"/>
       <c r="B115" s="10" t="s">
         <v>117</v>
       </c>
@@ -8008,7 +8008,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="75"/>
+      <c r="A116" s="80"/>
       <c r="B116" s="41" t="s">
         <v>118</v>
       </c>
@@ -8030,7 +8030,7 @@
       </c>
     </row>
     <row r="117" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="75"/>
+      <c r="A117" s="80"/>
       <c r="B117" s="41" t="s">
         <v>119</v>
       </c>
@@ -8052,7 +8052,7 @@
       </c>
     </row>
     <row r="118" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="75"/>
+      <c r="A118" s="80"/>
       <c r="B118" s="41" t="s">
         <v>120</v>
       </c>
@@ -8074,7 +8074,7 @@
       </c>
     </row>
     <row r="119" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="75"/>
+      <c r="A119" s="80"/>
       <c r="B119" s="41" t="s">
         <v>121</v>
       </c>
@@ -8096,7 +8096,7 @@
       </c>
     </row>
     <row r="120" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="75"/>
+      <c r="A120" s="80"/>
       <c r="B120" s="10" t="s">
         <v>122</v>
       </c>
@@ -8130,7 +8130,7 @@
       </c>
     </row>
     <row r="121" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="75"/>
+      <c r="A121" s="80"/>
       <c r="B121" s="43" t="s">
         <v>123</v>
       </c>
@@ -8152,7 +8152,7 @@
       </c>
     </row>
     <row r="122" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="75"/>
+      <c r="A122" s="80"/>
       <c r="B122" s="43" t="s">
         <v>124</v>
       </c>
@@ -8174,7 +8174,7 @@
       </c>
     </row>
     <row r="123" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="75"/>
+      <c r="A123" s="80"/>
       <c r="B123" s="43" t="s">
         <v>125</v>
       </c>
@@ -8196,7 +8196,7 @@
       </c>
     </row>
     <row r="124" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="75"/>
+      <c r="A124" s="80"/>
       <c r="B124" s="43" t="s">
         <v>126</v>
       </c>
@@ -8218,7 +8218,7 @@
       </c>
     </row>
     <row r="125" spans="1:10" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A125" s="75"/>
+      <c r="A125" s="80"/>
       <c r="B125" s="44" t="s">
         <v>127</v>
       </c>
@@ -8246,7 +8246,7 @@
       </c>
     </row>
     <row r="126" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="75"/>
+      <c r="A126" s="80"/>
       <c r="B126" s="41" t="s">
         <v>128</v>
       </c>
@@ -8268,7 +8268,7 @@
       </c>
     </row>
     <row r="127" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="75"/>
+      <c r="A127" s="80"/>
       <c r="B127" s="41" t="s">
         <v>129</v>
       </c>
@@ -8290,7 +8290,7 @@
       </c>
     </row>
     <row r="128" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="75"/>
+      <c r="A128" s="80"/>
       <c r="B128" s="41" t="s">
         <v>130</v>
       </c>
@@ -8312,7 +8312,7 @@
       </c>
     </row>
     <row r="129" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="75"/>
+      <c r="A129" s="80"/>
       <c r="B129" s="41" t="s">
         <v>131</v>
       </c>
@@ -8334,7 +8334,7 @@
       </c>
     </row>
     <row r="130" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="75"/>
+      <c r="A130" s="80"/>
       <c r="B130" s="41" t="s">
         <v>132</v>
       </c>
@@ -8356,7 +8356,7 @@
       </c>
     </row>
     <row r="131" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="75"/>
+      <c r="A131" s="80"/>
       <c r="B131" s="41" t="s">
         <v>133</v>
       </c>
@@ -8378,7 +8378,7 @@
       </c>
     </row>
     <row r="132" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="76"/>
+      <c r="A132" s="81"/>
       <c r="B132" s="57" t="s">
         <v>134</v>
       </c>
@@ -8400,7 +8400,7 @@
       </c>
     </row>
     <row r="133" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="74" t="s">
+      <c r="A133" s="79" t="s">
         <v>135</v>
       </c>
       <c r="B133" s="30" t="s">
@@ -8432,7 +8432,7 @@
       </c>
     </row>
     <row r="134" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="75"/>
+      <c r="A134" s="80"/>
       <c r="B134" s="49" t="s">
         <v>137</v>
       </c>
@@ -8454,7 +8454,7 @@
       </c>
     </row>
     <row r="135" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="75"/>
+      <c r="A135" s="80"/>
       <c r="B135" s="49" t="s">
         <v>138</v>
       </c>
@@ -8476,7 +8476,7 @@
       </c>
     </row>
     <row r="136" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="75"/>
+      <c r="A136" s="80"/>
       <c r="B136" s="49" t="s">
         <v>139</v>
       </c>
@@ -8498,7 +8498,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="75"/>
+      <c r="A137" s="80"/>
       <c r="B137" s="49" t="s">
         <v>140</v>
       </c>
@@ -8520,7 +8520,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="75"/>
+      <c r="A138" s="80"/>
       <c r="B138" s="49" t="s">
         <v>141</v>
       </c>
@@ -8542,7 +8542,7 @@
       </c>
     </row>
     <row r="139" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="75"/>
+      <c r="A139" s="80"/>
       <c r="B139" s="3" t="s">
         <v>142</v>
       </c>
@@ -8574,7 +8574,7 @@
       </c>
     </row>
     <row r="140" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="75"/>
+      <c r="A140" s="80"/>
       <c r="B140" s="41" t="s">
         <v>143</v>
       </c>
@@ -8596,7 +8596,7 @@
       </c>
     </row>
     <row r="141" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="75"/>
+      <c r="A141" s="80"/>
       <c r="B141" s="41" t="s">
         <v>144</v>
       </c>
@@ -8618,7 +8618,7 @@
       </c>
     </row>
     <row r="142" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="75"/>
+      <c r="A142" s="80"/>
       <c r="B142" s="41" t="s">
         <v>145</v>
       </c>
@@ -8640,7 +8640,7 @@
       </c>
     </row>
     <row r="143" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="75"/>
+      <c r="A143" s="80"/>
       <c r="B143" s="41" t="s">
         <v>146</v>
       </c>
@@ -8662,7 +8662,7 @@
       </c>
     </row>
     <row r="144" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="75"/>
+      <c r="A144" s="80"/>
       <c r="B144" s="41" t="s">
         <v>147</v>
       </c>
@@ -8684,7 +8684,7 @@
       </c>
     </row>
     <row r="145" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="75"/>
+      <c r="A145" s="80"/>
       <c r="B145" s="41" t="s">
         <v>148</v>
       </c>
@@ -8706,7 +8706,7 @@
       </c>
     </row>
     <row r="146" spans="1:10" collapsed="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="75"/>
+      <c r="A146" s="80"/>
       <c r="B146" s="9" t="s">
         <v>149</v>
       </c>
@@ -8736,7 +8736,7 @@
       </c>
     </row>
     <row r="147" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="75"/>
+      <c r="A147" s="80"/>
       <c r="B147" s="41" t="s">
         <v>150</v>
       </c>
@@ -8758,7 +8758,7 @@
       </c>
     </row>
     <row r="148" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="75"/>
+      <c r="A148" s="80"/>
       <c r="B148" s="41" t="s">
         <v>151</v>
       </c>
@@ -8780,7 +8780,7 @@
       </c>
     </row>
     <row r="149" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="75"/>
+      <c r="A149" s="80"/>
       <c r="B149" s="41" t="s">
         <v>152</v>
       </c>
@@ -8802,7 +8802,7 @@
       </c>
     </row>
     <row r="150" spans="1:10" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A150" s="76"/>
+      <c r="A150" s="81"/>
       <c r="B150" s="57" t="s">
         <v>153</v>
       </c>
@@ -8949,72 +8949,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="79"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="84"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="82"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="90"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88" t="s">
+      <c r="A4" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88" t="s">
+      <c r="F4" s="93"/>
+      <c r="G4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88" t="s">
+      <c r="H4" s="93"/>
+      <c r="I4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="106"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="113"/>
       <c r="C5" s="66" t="s">
         <v>175</v>
       </c>
@@ -9041,7 +9041,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="105" t="s">
+      <c r="A6" s="110" t="s">
         <v>158</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -9073,7 +9073,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="102"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="3" t="s">
         <v>160</v>
       </c>
@@ -9103,7 +9103,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="102"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="3" t="s">
         <v>163</v>
       </c>
@@ -9133,7 +9133,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="102"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
@@ -9163,7 +9163,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="102"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="3" t="s">
         <v>170</v>
       </c>
@@ -9193,7 +9193,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="102"/>
+      <c r="A11" s="107"/>
       <c r="B11" s="3" t="s">
         <v>43</v>
       </c>
@@ -9223,7 +9223,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="104"/>
+      <c r="A12" s="109"/>
       <c r="B12" s="24" t="s">
         <v>50</v>
       </c>
@@ -9253,7 +9253,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="110" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="28" t="s">
@@ -9285,7 +9285,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="102"/>
+      <c r="A14" s="107"/>
       <c r="B14" s="7" t="s">
         <v>65</v>
       </c>
@@ -9315,7 +9315,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="102"/>
+      <c r="A15" s="107"/>
       <c r="B15" s="7" t="s">
         <v>73</v>
       </c>
@@ -9345,7 +9345,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="102"/>
+      <c r="A16" s="107"/>
       <c r="B16" s="7" t="s">
         <v>78</v>
       </c>
@@ -9375,7 +9375,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="102"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="7" t="s">
         <v>88</v>
       </c>
@@ -9405,7 +9405,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="104"/>
+      <c r="A18" s="109"/>
       <c r="B18" s="29" t="s">
         <v>95</v>
       </c>
@@ -9435,7 +9435,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="79" t="s">
         <v>100</v>
       </c>
       <c r="B19" s="30" t="s">
@@ -9467,7 +9467,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="75"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="10" t="s">
         <v>103</v>
       </c>
@@ -9497,7 +9497,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="75"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="10" t="s">
         <v>106</v>
       </c>
@@ -9527,7 +9527,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="75"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="10" t="s">
         <v>111</v>
       </c>
@@ -9557,7 +9557,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="75"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="10" t="s">
         <v>117</v>
       </c>
@@ -9587,7 +9587,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="75"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="10" t="s">
         <v>122</v>
       </c>
@@ -9617,7 +9617,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="76"/>
+      <c r="A25" s="81"/>
       <c r="B25" s="26" t="s">
         <v>127</v>
       </c>
@@ -9647,7 +9647,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="79" t="s">
         <v>135</v>
       </c>
       <c r="B26" s="30" t="s">
@@ -9679,7 +9679,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="75"/>
+      <c r="A27" s="80"/>
       <c r="B27" s="3" t="s">
         <v>142</v>
       </c>
@@ -9709,7 +9709,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="75"/>
+      <c r="A28" s="80"/>
       <c r="B28" s="9" t="s">
         <v>184</v>
       </c>
@@ -9739,7 +9739,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="76"/>
+      <c r="A29" s="81"/>
       <c r="B29" s="31" t="s">
         <v>149</v>
       </c>
@@ -9847,14 +9847,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="114" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
@@ -9868,32 +9868,32 @@
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="110" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="112" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="112" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112" t="s">
+      <c r="A5" s="115" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="117" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112" t="s">
+      <c r="F5" s="117"/>
+      <c r="G5" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112" t="s">
+      <c r="H5" s="117"/>
+      <c r="I5" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="114"/>
+      <c r="J5" s="119"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="111"/>
-      <c r="B6" s="113"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="67" t="s">
         <v>175</v>
       </c>
@@ -9920,7 +9920,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="105" t="s">
+      <c r="A7" s="110" t="s">
         <v>158</v>
       </c>
       <c r="B7" s="19" t="s">
@@ -9952,7 +9952,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="102"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="3" t="s">
         <v>160</v>
       </c>
@@ -9982,7 +9982,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="102"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="3" t="s">
         <v>163</v>
       </c>
@@ -10012,7 +10012,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="102"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
@@ -10042,7 +10042,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="102"/>
+      <c r="A11" s="107"/>
       <c r="B11" s="3" t="s">
         <v>170</v>
       </c>
@@ -10072,7 +10072,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="102"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
@@ -10102,7 +10102,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="104"/>
+      <c r="A13" s="109"/>
       <c r="B13" s="24" t="s">
         <v>50</v>
       </c>
@@ -10132,7 +10132,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="110" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -10164,7 +10164,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="102"/>
+      <c r="A15" s="107"/>
       <c r="B15" s="7" t="s">
         <v>65</v>
       </c>
@@ -10194,7 +10194,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="102"/>
+      <c r="A16" s="107"/>
       <c r="B16" s="7" t="s">
         <v>73</v>
       </c>
@@ -10224,7 +10224,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="102"/>
+      <c r="A17" s="107"/>
       <c r="B17" s="7" t="s">
         <v>78</v>
       </c>
@@ -10254,7 +10254,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="102"/>
+      <c r="A18" s="107"/>
       <c r="B18" s="7" t="s">
         <v>88</v>
       </c>
@@ -10284,7 +10284,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="104"/>
+      <c r="A19" s="109"/>
       <c r="B19" s="29" t="s">
         <v>95</v>
       </c>
@@ -10314,7 +10314,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="79" t="s">
         <v>100</v>
       </c>
       <c r="B20" s="30" t="s">
@@ -10346,7 +10346,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="75"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="10" t="s">
         <v>103</v>
       </c>
@@ -10376,7 +10376,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="75"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="10" t="s">
         <v>106</v>
       </c>
@@ -10406,7 +10406,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="75"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="10" t="s">
         <v>111</v>
       </c>
@@ -10436,7 +10436,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A24" s="75"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="10" t="s">
         <v>117</v>
       </c>
@@ -10466,7 +10466,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A25" s="75"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="10" t="s">
         <v>122</v>
       </c>
@@ -10496,7 +10496,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="76"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="26" t="s">
         <v>127</v>
       </c>
@@ -10526,7 +10526,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="79" t="s">
         <v>135</v>
       </c>
       <c r="B27" s="30" t="s">
@@ -10558,7 +10558,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="75"/>
+      <c r="A28" s="80"/>
       <c r="B28" s="3" t="s">
         <v>142</v>
       </c>
@@ -10588,7 +10588,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="75"/>
+      <c r="A29" s="80"/>
       <c r="B29" s="9" t="s">
         <v>184</v>
       </c>
@@ -10618,7 +10618,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="76"/>
+      <c r="A30" s="81"/>
       <c r="B30" s="31" t="s">
         <v>149</v>
       </c>
@@ -10688,8 +10688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F969F0-3C06-441B-B708-8EBE32427589}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10697,49 +10697,49 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="82.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.81640625" style="127" customWidth="1"/>
+    <col min="4" max="5" width="11.81640625" style="78" customWidth="1"/>
     <col min="6" max="6" width="62.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="80.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="118"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="124"/>
     </row>
     <row r="2" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="34" t="s">
         <v>185</v>
       </c>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="125" t="s">
         <v>240</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="121"/>
+      <c r="C2" s="126"/>
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="127"/>
     </row>
     <row r="3" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="82"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="87"/>
     </row>
     <row r="4" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="89"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="90"/>
     </row>
     <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
@@ -10751,10 +10751,10 @@
       <c r="C5" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="123" t="s">
+      <c r="D5" s="74" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="74" t="s">
         <v>253</v>
       </c>
       <c r="F5" s="15" t="s">
@@ -10762,7 +10762,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="120" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="60" t="s">
@@ -10771,106 +10771,108 @@
       <c r="C6" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="124" t="s">
+      <c r="D6" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="124" t="s">
+      <c r="E6" s="75" t="s">
         <v>254</v>
       </c>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="115"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>192</v>
       </c>
       <c r="C7" s="61" t="s">
         <v>193</v>
       </c>
-      <c r="D7" s="124" t="s">
+      <c r="D7" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E7" s="124" t="s">
+      <c r="E7" s="75" t="s">
         <v>254</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="115"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="124" t="s">
+      <c r="D8" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E8" s="124" t="s">
-        <v>255</v>
+      <c r="E8" s="75" t="s">
+        <v>254</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="115"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D9" s="124" t="s">
+      <c r="D9" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E9" s="124" t="s">
-        <v>255</v>
+      <c r="E9" s="75" t="s">
+        <v>254</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="115"/>
+      <c r="A10" s="120"/>
       <c r="B10" s="16" t="s">
         <v>197</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="D10" s="124" t="s">
+      <c r="D10" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E10" s="124"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="115"/>
+      <c r="A11" s="120"/>
       <c r="B11" s="16" t="s">
         <v>199</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="124" t="s">
+      <c r="D11" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E11" s="124"/>
+      <c r="E11" s="75" t="s">
+        <v>255</v>
+      </c>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="115"/>
+      <c r="A12" s="120"/>
       <c r="B12" s="16" t="s">
         <v>201</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="D12" s="124" t="s">
+      <c r="D12" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E12" s="124"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="115" t="s">
+      <c r="A13" s="120" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -10879,124 +10881,122 @@
       <c r="C13" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="D13" s="124" t="s">
+      <c r="D13" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E13" s="124"/>
+      <c r="E13" s="75"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="115"/>
+      <c r="A14" s="120"/>
       <c r="B14" s="60" t="s">
         <v>205</v>
       </c>
       <c r="C14" s="61" t="s">
         <v>206</v>
       </c>
-      <c r="D14" s="124" t="s">
+      <c r="D14" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="124"/>
+      <c r="E14" s="75"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="115"/>
+      <c r="A15" s="120"/>
       <c r="B15" s="16" t="s">
         <v>207</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D15" s="124" t="s">
+      <c r="D15" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E15" s="124" t="s">
+      <c r="E15" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="116" x14ac:dyDescent="0.35">
-      <c r="A16" s="115"/>
+      <c r="A16" s="120"/>
       <c r="B16" s="60" t="s">
         <v>208</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>209</v>
       </c>
-      <c r="D16" s="124" t="s">
+      <c r="D16" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E16" s="124" t="s">
+      <c r="E16" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="115"/>
+      <c r="A17" s="120"/>
       <c r="B17" s="17" t="s">
         <v>210</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="124" t="s">
+      <c r="D17" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E17" s="124" t="s">
+      <c r="E17" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A18" s="115"/>
+      <c r="A18" s="120"/>
       <c r="B18" s="60" t="s">
         <v>212</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>213</v>
       </c>
-      <c r="D18" s="124" t="s">
+      <c r="D18" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E18" s="124" t="s">
+      <c r="E18" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="115"/>
+      <c r="A19" s="120"/>
       <c r="B19" s="60" t="s">
         <v>214</v>
       </c>
       <c r="C19" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E19" s="124" t="s">
-        <v>256</v>
-      </c>
+      <c r="E19" s="75"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="115"/>
+      <c r="A20" s="120"/>
       <c r="B20" s="60" t="s">
         <v>216</v>
       </c>
       <c r="C20" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="D20" s="125" t="s">
+      <c r="D20" s="76" t="s">
         <v>191</v>
       </c>
-      <c r="E20" s="124" t="s">
-        <v>256</v>
+      <c r="E20" s="75" t="s">
+        <v>255</v>
       </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="115" t="s">
+      <c r="A21" s="120" t="s">
         <v>100</v>
       </c>
       <c r="B21" s="60" t="s">
@@ -11005,162 +11005,162 @@
       <c r="C21" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="124" t="s">
+      <c r="D21" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E21" s="124"/>
+      <c r="E21" s="75"/>
       <c r="F21" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="115"/>
+      <c r="A22" s="120"/>
       <c r="B22" s="60" t="s">
         <v>220</v>
       </c>
       <c r="C22" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="D22" s="124" t="s">
+      <c r="D22" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E22" s="124"/>
+      <c r="E22" s="75"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="115"/>
+      <c r="A23" s="120"/>
       <c r="B23" s="60" t="s">
         <v>111</v>
       </c>
       <c r="C23" s="61" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="124" t="s">
+      <c r="D23" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E23" s="124"/>
+      <c r="E23" s="75"/>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="115"/>
+      <c r="A24" s="120"/>
       <c r="B24" s="60" t="s">
         <v>223</v>
       </c>
       <c r="C24" s="61"/>
-      <c r="D24" s="124" t="s">
+      <c r="D24" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E24" s="124"/>
+      <c r="E24" s="75"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="115"/>
+      <c r="A25" s="120"/>
       <c r="B25" s="60" t="s">
         <v>106</v>
       </c>
       <c r="C25" s="61" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="124" t="s">
+      <c r="D25" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E25" s="124"/>
+      <c r="E25" s="75"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="115"/>
+      <c r="A26" s="120"/>
       <c r="B26" s="16" t="s">
         <v>127</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D26" s="124" t="s">
+      <c r="D26" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="E26" s="124" t="s">
+      <c r="E26" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="115"/>
+      <c r="A27" s="120"/>
       <c r="B27" s="16" t="s">
         <v>226</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="D27" s="124" t="s">
+      <c r="D27" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="124"/>
+      <c r="E27" s="75"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="115"/>
+      <c r="A28" s="120"/>
       <c r="B28" s="16" t="s">
         <v>228</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="126" t="s">
+      <c r="D28" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="E28" s="126"/>
+      <c r="E28" s="77"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A29" s="115" t="s">
+      <c r="A29" s="120" t="s">
         <v>229</v>
       </c>
       <c r="B29" s="60" t="s">
         <v>230</v>
       </c>
       <c r="C29" s="60"/>
-      <c r="D29" s="125" t="s">
+      <c r="D29" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="E29" s="125"/>
+      <c r="E29" s="76"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="115"/>
+      <c r="A30" s="120"/>
       <c r="B30" s="60" t="s">
         <v>231</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="126" t="s">
+      <c r="D30" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="E30" s="126"/>
+      <c r="E30" s="77"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="115"/>
+      <c r="A31" s="120"/>
       <c r="B31" s="60" t="s">
         <v>232</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="126" t="s">
+      <c r="D31" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="E31" s="126"/>
+      <c r="E31" s="77"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="115"/>
+      <c r="A32" s="120"/>
       <c r="B32" s="60" t="s">
         <v>233</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="126" t="s">
+      <c r="D32" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="E32" s="126"/>
+      <c r="E32" s="77"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="115" t="s">
+      <c r="A33" s="120" t="s">
         <v>234</v>
       </c>
       <c r="B33" s="60" t="s">
@@ -11169,26 +11169,26 @@
       <c r="C33" s="61" t="s">
         <v>236</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="75" t="s">
         <v>191</v>
       </c>
-      <c r="E33" s="124" t="s">
+      <c r="E33" s="75" t="s">
         <v>256</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="115"/>
+      <c r="A34" s="120"/>
       <c r="B34" s="16" t="s">
         <v>237</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D34" s="126" t="s">
+      <c r="D34" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="E34" s="126"/>
+      <c r="E34" s="77"/>
       <c r="F34" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>